<commit_message>
add new benchmark result
</commit_message>
<xml_diff>
--- a/synquid/test/succinct/synquid_benchmark.xlsx
+++ b/synquid/test/succinct/synquid_benchmark.xlsx
@@ -346,6 +346,1893 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$1:$A$91</c:f>
+              <c:strCache>
+                <c:ptCount val="91"/>
+                <c:pt idx="0">
+                  <c:v>AVL-BalL0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>AVL-BalLL</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>AVL-BalLR</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>AVL-BalR0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>AVL-BalRL</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>AVL-BalRR</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>AVL-Balance</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>AVL-Insert</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>AVL-ExtractMin</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>AVL-Delete</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>RBT-BalanceL</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>RBT-BalanceR</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>RBT-Insert</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>List-Zip</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>List-Zip3</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>List-Zip4</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>List-Zip5</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>List-Zip6</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>Graph-Weighted</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>Graph-Colored</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>Graph-Labeled</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>BST-Delete-T2</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>BST-Delete-T2-1</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>BST-Delete-T2-2</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>BST-Delete-T2-3</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>BST-Delete-T2-4</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>BST-Delete-T2-5</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>BST-Delete-T2-6</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>BST-Delete-T2-7</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>BST-Delete-T2-8</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>BST-Delete-T2-9</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>BST-Delete-T3</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>Int-Max2</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>Int-Max3</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>Int-Max4</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>Int-Max5</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>Array-Search-2</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>Array-Search-3</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>Array-Search-4</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>Array-Search-5</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>Array-Search-6</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>Int-Add</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>List-Null</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>List-Elem</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>List-Stutter</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>List-Replicate</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>List-Append</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>List-Concat</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>List-Take</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>List-Drop</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>List-Delete</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>List-Map</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>List-ZipWith</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>List-Zip</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>List-ToNat</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>List-Product</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>List-ExtractMin</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>List-Intersection</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>List-Fold</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>List-Fold-Length</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>List-Fold-Append</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>List-Ith</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>List-ElemIndex</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>List-Snoc</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>List-Reverse</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>UniqueList-Insert</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>UniqueList-Delete</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>UniqueList-Range</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>List-Nub</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>List-Compress</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>List-InsertSort</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>List-Fold-Sort</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>List-Split</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>IncList-Merge</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>IncList-MergeSort</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>List-Partition</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>IncList-PivotAppend</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>IncList-QuickSort</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>Tree-Elem</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>Tree-Flatten</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>BST-Member</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>BST-Insert</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>BST-ExtractMin</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>BST-Delete</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>BST-Sort</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>BinHeap-Member</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>BinHeap-Insert</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>Evaluator</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>AddressBook-Make</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>AddressBook-Merge</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>Replicate-Examples</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$1:$B$91</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="91"/>
+                <c:pt idx="0">
+                  <c:v>1.41</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.2300000000000004</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8.76</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.1100000000000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>9.0399999999999991</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6.71</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6.15</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.89</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>5.72</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>27.78</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>96.85</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>79.97</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>16.77</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.53</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0.48</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>0.62</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>1.42</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>9.6</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>0.49</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>0.86</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>1.81</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>4.54</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>11.92</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>1.1599999999999999</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>0.44</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>0.49</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>0.51</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>0.45</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>0.52</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>0.54</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>0.57999999999999996</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>0.49</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>0.65</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>0.53</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>0.49</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>6.35</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>7.43</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>2.58</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>0.77</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>0.52</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>0.55000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>0.47</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>0.68</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>0.56999999999999995</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>0.52</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>0.56000000000000005</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>0.56999999999999995</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>1.7</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>0.95</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>1.84</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>0.82</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>2.17</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>1.72</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>3.61</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>3.49</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>10.78</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>1.06</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>5.15</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>2.73</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>0.55000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>0.53</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>0.93</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>10.59</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>4.24</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>1.73</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>2.91</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>0.94</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>15.81</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>1.22</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>1.1499999999999999</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>0.5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-8ED3-4E62-8BDE-D06EE207A396}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$1:$A$91</c:f>
+              <c:strCache>
+                <c:ptCount val="91"/>
+                <c:pt idx="0">
+                  <c:v>AVL-BalL0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>AVL-BalLL</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>AVL-BalLR</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>AVL-BalR0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>AVL-BalRL</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>AVL-BalRR</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>AVL-Balance</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>AVL-Insert</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>AVL-ExtractMin</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>AVL-Delete</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>RBT-BalanceL</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>RBT-BalanceR</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>RBT-Insert</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>List-Zip</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>List-Zip3</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>List-Zip4</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>List-Zip5</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>List-Zip6</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>Graph-Weighted</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>Graph-Colored</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>Graph-Labeled</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>BST-Delete-T2</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>BST-Delete-T2-1</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>BST-Delete-T2-2</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>BST-Delete-T2-3</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>BST-Delete-T2-4</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>BST-Delete-T2-5</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>BST-Delete-T2-6</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>BST-Delete-T2-7</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>BST-Delete-T2-8</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>BST-Delete-T2-9</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>BST-Delete-T3</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>Int-Max2</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>Int-Max3</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>Int-Max4</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>Int-Max5</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>Array-Search-2</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>Array-Search-3</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>Array-Search-4</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>Array-Search-5</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>Array-Search-6</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>Int-Add</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>List-Null</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>List-Elem</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>List-Stutter</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>List-Replicate</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>List-Append</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>List-Concat</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>List-Take</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>List-Drop</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>List-Delete</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>List-Map</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>List-ZipWith</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>List-Zip</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>List-ToNat</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>List-Product</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>List-ExtractMin</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>List-Intersection</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>List-Fold</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>List-Fold-Length</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>List-Fold-Append</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>List-Ith</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>List-ElemIndex</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>List-Snoc</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>List-Reverse</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>UniqueList-Insert</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>UniqueList-Delete</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>UniqueList-Range</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>List-Nub</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>List-Compress</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>List-InsertSort</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>List-Fold-Sort</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>List-Split</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>IncList-Merge</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>IncList-MergeSort</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>List-Partition</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>IncList-PivotAppend</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>IncList-QuickSort</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>Tree-Elem</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>Tree-Flatten</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>BST-Member</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>BST-Insert</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>BST-ExtractMin</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>BST-Delete</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>BST-Sort</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>BinHeap-Member</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>BinHeap-Insert</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>Evaluator</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>AddressBook-Make</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>AddressBook-Merge</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>Replicate-Examples</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$C$1:$C$91</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="91"/>
+                <c:pt idx="0">
+                  <c:v>1.33</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.92</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8.1300000000000008</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.01</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7.47</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>11.6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3.46</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4.12</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>5.73</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>34.68</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>31.11</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>49.18</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>15.88</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.72</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0.47</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>0.55000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>1.1000000000000001</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>8.0299999999999994</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>0.51</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>0.66</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>1.07</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>2.0699999999999998</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>4.68</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>2.5299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>0.48</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>0.54</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>0.52</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>0.63</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>0.57999999999999996</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>0.62</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>0.52</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>0.72</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>1.56</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>9.8699999999999992</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>5.19</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>0.68</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>0.47</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>0.71</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>0.56000000000000005</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>0.65</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>0.64</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>0.59</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>0.79</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>0.85</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>4.88</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>2.9</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>2.2799999999999998</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>1.29</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>3.22</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>2.0499999999999998</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>4.92</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>3.98</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>20.56</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>1.02</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>4.62</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>0.91</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>0.77</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>0.56000000000000005</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>1.85</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>17.190000000000001</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>12.35</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>2.5</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>1.06</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>1.25</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>1.9</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>1.32</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>1.26</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>0.65</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-8ED3-4E62-8BDE-D06EE207A396}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="392642600"/>
+        <c:axId val="392642928"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="392642600"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="392642928"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="392642928"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="392642600"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>187324</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>146050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>222249</xdr:colOff>
+      <xdr:row>86</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F9DE50AE-CA98-46B6-AEC9-F32C2DC649CE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -645,10 +2532,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B91"/>
+  <dimension ref="A1:C91"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="B75" sqref="B75"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -656,124 +2543,166 @@
     <col min="1" max="1" width="17.90625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1">
         <v>1.41</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C1">
+        <v>1.33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>1</v>
       </c>
       <c r="B2">
         <v>4.2300000000000004</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C2">
+        <v>5.92</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>2</v>
       </c>
       <c r="B3">
         <v>8.76</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C3">
+        <v>8.1300000000000008</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>3</v>
       </c>
       <c r="B4">
         <v>1.1100000000000001</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C4">
+        <v>1.01</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>4</v>
       </c>
       <c r="B5">
         <v>9.0399999999999991</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C5">
+        <v>7.47</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>5</v>
       </c>
       <c r="B6">
         <v>6.71</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C6">
+        <v>11.6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>6</v>
       </c>
       <c r="B7">
         <v>6.15</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C7">
+        <v>3.46</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>7</v>
       </c>
       <c r="B8">
         <v>2.89</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C8">
+        <v>4.12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>8</v>
       </c>
       <c r="B9">
         <v>5.72</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C9">
+        <v>5.73</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>9</v>
       </c>
       <c r="B10">
         <v>27.78</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C10">
+        <v>34.68</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>10</v>
       </c>
       <c r="B11">
         <v>96.85</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C11">
+        <v>31.11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>11</v>
       </c>
       <c r="B12">
         <v>79.97</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C12">
+        <v>49.18</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>12</v>
       </c>
       <c r="B13">
         <v>16.77</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C13">
+        <v>15.88</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>13</v>
       </c>
       <c r="B14">
         <v>0.53</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C14">
+        <v>0.72</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>15</v>
       </c>
@@ -858,479 +2787,657 @@
         <v>31</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>32</v>
       </c>
       <c r="B33">
         <v>0.48</v>
       </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C33">
+        <v>0.47</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>33</v>
       </c>
       <c r="B34">
         <v>0.62</v>
       </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C34">
+        <v>0.55000000000000004</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>34</v>
       </c>
       <c r="B35">
         <v>1.42</v>
       </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C35">
+        <v>1.1000000000000001</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>35</v>
       </c>
       <c r="B36">
         <v>9.6</v>
       </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C36">
+        <v>8.0299999999999994</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>36</v>
       </c>
       <c r="B37">
         <v>0.49</v>
       </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C37">
+        <v>0.51</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>37</v>
       </c>
       <c r="B38">
         <v>0.86</v>
       </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C38">
+        <v>0.66</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>38</v>
       </c>
       <c r="B39">
         <v>1.81</v>
       </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C39">
+        <v>1.07</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>39</v>
       </c>
       <c r="B40">
         <v>4.54</v>
       </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C40">
+        <v>2.0699999999999998</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>40</v>
       </c>
       <c r="B41">
         <v>11.92</v>
       </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C41">
+        <v>4.68</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>41</v>
       </c>
       <c r="B42">
         <v>1.1599999999999999</v>
       </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C42">
+        <v>2.5299999999999998</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>42</v>
       </c>
       <c r="B43">
         <v>0.44</v>
       </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C43">
+        <v>0.48</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>43</v>
       </c>
       <c r="B44">
         <v>0.49</v>
       </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C44">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>44</v>
       </c>
       <c r="B45">
         <v>0.51</v>
       </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C45">
+        <v>0.54</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>45</v>
       </c>
       <c r="B46">
         <v>0.45</v>
       </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C46">
+        <v>0.52</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>46</v>
       </c>
       <c r="B47">
         <v>0.7</v>
       </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C47">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>47</v>
       </c>
       <c r="B48">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C48">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>48</v>
       </c>
       <c r="B49">
         <v>0.52</v>
       </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C49">
+        <v>0.63</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>49</v>
       </c>
       <c r="B50">
         <v>0.54</v>
       </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C50">
+        <v>0.57999999999999996</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>50</v>
       </c>
       <c r="B51">
         <v>0.57999999999999996</v>
       </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C51">
+        <v>0.62</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>51</v>
       </c>
       <c r="B52">
         <v>0.49</v>
       </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C52">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>52</v>
       </c>
       <c r="B53">
         <v>0.65</v>
       </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C53">
+        <v>0.52</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>13</v>
       </c>
       <c r="B54">
         <v>0.53</v>
       </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C54">
+        <v>0.72</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>53</v>
       </c>
       <c r="B55">
         <v>0.49</v>
       </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C55">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>54</v>
       </c>
       <c r="B56">
         <v>6.35</v>
       </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C56">
+        <v>1.56</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
         <v>55</v>
       </c>
       <c r="B57">
         <v>7.43</v>
       </c>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C57">
+        <v>9.8699999999999992</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
         <v>56</v>
       </c>
       <c r="B58">
         <v>2.58</v>
       </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C58">
+        <v>5.19</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
         <v>57</v>
       </c>
       <c r="B59">
         <v>0.77</v>
       </c>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C59">
+        <v>0.68</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
         <v>58</v>
       </c>
       <c r="B60">
         <v>0.52</v>
       </c>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C60">
+        <v>0.47</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
         <v>59</v>
       </c>
       <c r="B61">
         <v>0.55000000000000004</v>
       </c>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C61">
+        <v>0.71</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
         <v>60</v>
       </c>
       <c r="B62">
         <v>0.47</v>
       </c>
-    </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C62">
+        <v>0.56000000000000005</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
         <v>61</v>
       </c>
       <c r="B63">
         <v>0.68</v>
       </c>
-    </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C63">
+        <v>0.65</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
         <v>62</v>
       </c>
       <c r="B64">
         <v>0.56999999999999995</v>
       </c>
-    </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C64">
+        <v>0.64</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
         <v>63</v>
       </c>
       <c r="B65">
         <v>0.52</v>
       </c>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C65">
+        <v>0.59</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
         <v>64</v>
       </c>
       <c r="B66">
         <v>0.56000000000000005</v>
       </c>
-    </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C66">
+        <v>0.79</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
         <v>65</v>
       </c>
       <c r="B67">
         <v>0.56999999999999995</v>
       </c>
-    </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C67">
+        <v>0.85</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
         <v>66</v>
       </c>
       <c r="B68">
         <v>1.7</v>
       </c>
-    </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C68">
+        <v>4.88</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
         <v>67</v>
       </c>
       <c r="B69">
         <v>0.95</v>
       </c>
-    </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C69">
+        <v>2.9</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
         <v>68</v>
       </c>
       <c r="B70">
         <v>1.84</v>
       </c>
-    </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C70">
+        <v>2.2799999999999998</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
         <v>69</v>
       </c>
       <c r="B71">
         <v>0.82</v>
       </c>
-    </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C71">
+        <v>1.29</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
         <v>70</v>
       </c>
       <c r="B72">
         <v>2.17</v>
       </c>
-    </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C72">
+        <v>3.22</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
         <v>71</v>
       </c>
       <c r="B73">
         <v>1.72</v>
       </c>
-    </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C73">
+        <v>2.0499999999999998</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
         <v>72</v>
       </c>
       <c r="B74">
         <v>3.61</v>
       </c>
-    </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C74">
+        <v>4.92</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
         <v>73</v>
       </c>
       <c r="B75">
         <v>3.49</v>
       </c>
-    </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C75">
+        <v>3.98</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
         <v>74</v>
       </c>
       <c r="B76">
         <v>10.78</v>
       </c>
-    </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C76">
+        <v>20.56</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
         <v>75</v>
       </c>
       <c r="B77">
         <v>1.06</v>
       </c>
-    </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C77">
+        <v>1.02</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
         <v>76</v>
       </c>
       <c r="B78">
         <v>5.15</v>
       </c>
-    </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C78">
+        <v>4.62</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
         <v>77</v>
       </c>
       <c r="B79">
         <v>2.73</v>
       </c>
-    </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C79">
+        <v>0.91</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
         <v>78</v>
       </c>
       <c r="B80">
         <v>0.55000000000000004</v>
       </c>
-    </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C80">
+        <v>0.77</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
         <v>79</v>
       </c>
       <c r="B81">
         <v>0.53</v>
       </c>
-    </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C81">
+        <v>0.56000000000000005</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
         <v>80</v>
       </c>
       <c r="B82">
         <v>0.93</v>
       </c>
-    </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C82">
+        <v>1.85</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
         <v>81</v>
       </c>
       <c r="B83">
         <v>10.59</v>
       </c>
-    </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C83">
+        <v>17.190000000000001</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
         <v>82</v>
       </c>
       <c r="B84">
         <v>4.24</v>
       </c>
-    </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C84">
+        <v>12.35</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
         <v>83</v>
       </c>
       <c r="B85">
         <v>1.73</v>
       </c>
-    </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C85">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
         <v>84</v>
       </c>
       <c r="B86">
         <v>2.91</v>
       </c>
-    </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C86">
+        <v>1.06</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
         <v>85</v>
       </c>
       <c r="B87">
         <v>0.94</v>
       </c>
-    </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C87">
+        <v>1.25</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
         <v>86</v>
       </c>
       <c r="B88">
         <v>15.81</v>
       </c>
-    </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C88">
+        <v>1.9</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
         <v>87</v>
       </c>
       <c r="B89">
         <v>1.22</v>
       </c>
-    </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C89">
+        <v>1.32</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
         <v>88</v>
       </c>
       <c r="B90">
         <v>1.1499999999999999</v>
       </c>
-    </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C90">
+        <v>1.26</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
         <v>89</v>
       </c>
       <c r="B91">
         <v>0.5</v>
       </c>
+      <c r="C91">
+        <v>0.65</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>